<commit_message>
fixed multiplier table lookup
</commit_message>
<xml_diff>
--- a/test_problem/swmm.xlsx
+++ b/test_problem/swmm.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-3140" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-76820" yWindow="-7960" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -3250,7 +3250,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3273,6 +3276,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF454545"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -3299,13 +3308,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -5957,13 +5967,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:OK429"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="NM1" workbookViewId="0">
-      <selection activeCell="OI7" sqref="OI7"/>
+    <sheetView tabSelected="1" topLeftCell="LP1" workbookViewId="0">
+      <selection activeCell="LZ14" sqref="LZ14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="338" max="338" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:401" x14ac:dyDescent="0.2">
@@ -8614,6 +8625,9 @@
       </c>
       <c r="K14">
         <v>38.5471</v>
+      </c>
+      <c r="LZ14" s="4">
+        <v>42495.40625</v>
       </c>
     </row>
     <row r="15" spans="1:401" x14ac:dyDescent="0.2">

</xml_diff>